<commit_message>
fomrat 2 backend done
</commit_message>
<xml_diff>
--- a/f1.xlsx
+++ b/f1.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -825,458 +825,402 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B56">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B57">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B58">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B59">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="B60">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B61">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B62">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B63">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="B64">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B66">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B67">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B68">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B69">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B70">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B71">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B72">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B73">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B74">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B75">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B76">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B77">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B78">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B79">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="B80">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B81">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B82">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B83">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B84">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B85">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B86">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B87">
-        <v>94</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B88">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B89">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B90">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B91">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
+        <v>49</v>
+      </c>
+      <c r="B92">
         <v>80</v>
-      </c>
-      <c r="B92">
-        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B93">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B94">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B95">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B96">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B97">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B98">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B99">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B100">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B101">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B102">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B103">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B104">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B105">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106">
-        <v>65</v>
-      </c>
-      <c r="B106">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107">
-        <v>58</v>
-      </c>
-      <c r="B107">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108">
-        <v>62</v>
-      </c>
-      <c r="B108">
         <v>67</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109">
-        <v>50</v>
-      </c>
-      <c r="B109">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110">
-        <v>74</v>
-      </c>
-      <c r="B110">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111">
-        <v>49</v>
-      </c>
-      <c r="B111">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112">
-        <v>28</v>
-      </c>
-      <c r="B112">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>